<commit_message>
adicionar os botoes de assinatura com delay
</commit_message>
<xml_diff>
--- a/agrupado.xlsx
+++ b/agrupado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,12 +478,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2839.91</t>
+          <t>83.79</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>200.21</t>
+          <t>5.91</t>
         </is>
       </c>
     </row>
@@ -505,19 +505,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>408.09</t>
+          <t>119.79</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>28.76</t>
+          <t>8.45</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>00758606000190</t>
+          <t>00437311000112</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,19 +532,19 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>239800.00</t>
+          <t>144210.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>22661.12</t>
+          <t>13627.84</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>00948060000130</t>
+          <t>00449936000102</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -559,73 +559,73 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7749.00</t>
+          <t>17272.96</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>453.32</t>
+          <t>1010.47</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00948060000130</t>
+          <t>00462284000138</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>17003</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>54568.00</t>
+          <t>830.89</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>5156.68</t>
+          <t>10.30</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01459413000100</t>
+          <t>01016052000119</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6484.28</t>
+          <t>1677.00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>612.76</t>
+          <t>98.10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01568077000206</t>
+          <t>01016052000119</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -640,147 +640,147 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>24016.52</t>
+          <t>370.00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2269.56</t>
+          <t>34.96</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02012862000160</t>
+          <t>01437983000271</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>29473.00</t>
+          <t>1840.00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>294.70</t>
+          <t>107.64</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>02012862000160</t>
+          <t>01437983000271</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6256</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>29473.00</t>
+          <t>120.00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>707.35</t>
+          <t>11.34</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02012862000160</t>
+          <t>01498154000118</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>8850</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17072.60</t>
+          <t>6186.67</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>580.48</t>
+          <t>76.71</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>02012862001131</t>
+          <t>01568077000206</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>69466.68</t>
+          <t>51072.04</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>694.67</t>
+          <t>4826.31</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>02012862001131</t>
+          <t>01781573000162</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17032</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>35345.10</t>
+          <t>459327.06</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>353.45</t>
+          <t>43406.41</t>
         </is>
       </c>
     </row>
@@ -792,7 +792,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>6256</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -802,12 +802,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>69466.68</t>
+          <t>33190.90</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1667.20</t>
+          <t>331.91</t>
         </is>
       </c>
     </row>
@@ -824,71 +824,71 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>35345.10</t>
+          <t>33190.90</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>848.28</t>
+          <t>796.58</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>02604236000162</t>
+          <t>02355633000148</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2900.00</t>
+          <t>1524.96</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>169.65</t>
+          <t>144.11</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>02846056000197</t>
+          <t>02604236000162</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2317.50</t>
+          <t>6200.00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>163.40</t>
+          <t>362.70</t>
         </is>
       </c>
     </row>
@@ -905,326 +905,326 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>168.02</t>
+          <t>43.29</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>11.84</t>
+          <t>3.05</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03746938001387</t>
+          <t>03281744000110</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17003</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>41430.50</t>
+          <t>570.89</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2423.68</t>
+          <t>7.08</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04539534000141</t>
+          <t>03701024000166</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17033</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>23161.22</t>
+          <t>122.35</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2188.74</t>
+          <t>1.52</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05111625000144</t>
+          <t>04168835000106</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1071.00</t>
+          <t>421.85</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>62.65</t>
+          <t>5.23</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>07179175000157</t>
+          <t>04409762000440</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6175</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>16087.00</t>
+          <t>37.02</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>941.09</t>
+          <t>2.61</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>07575651002950</t>
+          <t>04900474000140</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17032</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>86388.10</t>
+          <t>231542.18</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>863.87</t>
+          <t>21880.74</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>07575651002950</t>
+          <t>05111625000144</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>30602.00</t>
+          <t>1200.00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>306.02</t>
+          <t>70.20</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>07575651002950</t>
+          <t>05202938000108</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6256</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>91814.80</t>
+          <t>287434.70</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2203.51</t>
+          <t>16814.93</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>07575651002950</t>
+          <t>06088039000199</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6256</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17001</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>30602.00</t>
+          <t>226252.12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>734.45</t>
+          <t>13235.75</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>07575881000118</t>
+          <t>06212140000290</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>26070.58</t>
+          <t>612.58</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2463.66</t>
+          <t>7.60</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>08735199000108</t>
+          <t>07063185000203</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>17033</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>25191.26</t>
+          <t>185.10</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2380.57</t>
+          <t>2.30</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>08772204000152</t>
+          <t>07575651002950</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1794.90</t>
+          <t>27280.56</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>105.00</t>
+          <t>272.81</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>09296295000160</t>
+          <t>07575651002950</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6256</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1234,24 +1234,24 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>306843.50</t>
+          <t>27280.56</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3068.39</t>
+          <t>654.73</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>09296295000160</t>
+          <t>07575881000118</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1261,127 +1261,127 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>40054.00</t>
+          <t>10467.63</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>400.54</t>
+          <t>989.19</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>09296295000160</t>
+          <t>07594533000198</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6256</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>301416.80</t>
+          <t>20540.59</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>7234.01</t>
+          <t>254.70</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>09296295000160</t>
+          <t>07674744000130</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6256</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>40054.00</t>
+          <t>6210.00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>961.30</t>
+          <t>586.84</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>10486051000129</t>
+          <t>07774050000175</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17031</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>46800.00</t>
+          <t>8223617.76</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2737.80</t>
+          <t>777131.88</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>11319557000378</t>
+          <t>07859130000123</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1760.00</t>
+          <t>447.09</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>102.96</t>
+          <t>5.54</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>11533627000124</t>
+          <t>07999951000165</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1391,861 +1391,861 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17033</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>61386.72</t>
+          <t>1800.00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3591.12</t>
+          <t>105.30</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>12467682000126</t>
+          <t>08072308000316</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>18150.00</t>
+          <t>2132.12</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1061.79</t>
+          <t>26.44</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>13498023000110</t>
+          <t>08072308000669</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>17003</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4287.14</t>
+          <t>491.31</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>250.80</t>
+          <t>6.09</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>13498023000110</t>
+          <t>08374804000162</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>17004</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>131121.64</t>
+          <t>32781.00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>7670.60</t>
+          <t>3097.80</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>14208934000128</t>
+          <t>08399834000123</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>17004</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3377.95</t>
+          <t>732.79</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>197.61</t>
+          <t>9.09</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>14522178000107</t>
+          <t>08418303000130</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>140.10</t>
+          <t>474.75</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>9.90</t>
+          <t>5.89</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>14522178000107</t>
+          <t>08638541000151</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>115.40</t>
+          <t>15309.00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>8.13</t>
+          <t>895.57</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>14639720000106</t>
+          <t>08735199000108</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17033</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>217.62</t>
+          <t>50382.52</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>15.36</t>
+          <t>4761.14</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>14639720000106</t>
+          <t>09047230000180</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>72.54</t>
+          <t>269.25</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>5.11</t>
+          <t>3.34</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>15150504000165</t>
+          <t>09296295000160</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>17033</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>76101.02</t>
+          <t>74444.44</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>7191.55</t>
+          <t>744.46</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>15559082000186</t>
+          <t>09296295000160</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>436.95</t>
+          <t>10319.40</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>30.80</t>
+          <t>103.19</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>15559082000186</t>
+          <t>09296295000160</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6256</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>236.08</t>
+          <t>74444.54</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>16.64</t>
+          <t>1786.67</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>15578569000106</t>
+          <t>09296295000160</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6256</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2822.59</t>
+          <t>10319.40</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>199.00</t>
+          <t>247.67</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>15578569000106</t>
+          <t>09422042000195</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17032</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>91.95</t>
+          <t>59903.74</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>6.48</t>
+          <t>5660.90</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>16951665000110</t>
+          <t>09422042000195</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17033</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>297.00</t>
+          <t>41749.42</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>17.38</t>
+          <t>3945.32</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>16951665000110</t>
+          <t>09445502000109</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17032</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2660.00</t>
+          <t>1006472.97</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>251.37</t>
+          <t>58878.67</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>17846647000131</t>
+          <t>09533651000111</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6188</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3841.80</t>
+          <t>189.59</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>270.84</t>
+          <t>2.35</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>18301321000191</t>
+          <t>09571844000167</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>17033</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>9006.63</t>
+          <t>343.91</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>851.13</t>
+          <t>4.26</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19674909000153</t>
+          <t>10530701000196</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>435.15</t>
+          <t>1089.89</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>30.70</t>
+          <t>13.51</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19674909000153</t>
+          <t>10641724000178</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>121.60</t>
+          <t>73.20</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>8.57</t>
+          <t>4.28</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19726111000108</t>
+          <t>10835932000108</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17002</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>680.60</t>
+          <t>2787260.36</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>47.99</t>
+          <t>182625.62</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>19726111000108</t>
+          <t>10996148000181</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>41.80</t>
+          <t>771.63</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2.94</t>
+          <t>9.57</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>21563512000136</t>
+          <t>11319557000378</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>219.55</t>
+          <t>76071.28</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>15.50</t>
+          <t>4450.17</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>27059460000141</t>
+          <t>11533627000124</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17003</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>50.83</t>
+          <t>1214204.77</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>3.58</t>
+          <t>71030.98</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>27059565000109</t>
+          <t>11601184000242</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>199.28</t>
+          <t>595.63</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>14.04</t>
+          <t>7.39</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>27729308000129</t>
+          <t>11642408000183</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>17001</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3652.56</t>
+          <t>451.46</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>213.67</t>
+          <t>5.60</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>27729308000129</t>
+          <t>11694577000671</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3445.00</t>
+          <t>29522.34</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>201.53</t>
+          <t>366.08</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>27950582000123</t>
+          <t>11963931000101</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>606.90</t>
+          <t>343.03</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>42.75</t>
+          <t>4.25</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>28388260000103</t>
+          <t>12035234000153</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17001</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>232.85</t>
+          <t>12917.46</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>16.40</t>
+          <t>1220.70</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>28388260000103</t>
+          <t>12396339000308</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>17099</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>230.03</t>
+          <t>264.65</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>16.21</t>
+          <t>3.28</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>28820255000110</t>
+          <t>12467682000126</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8767</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>17021</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>12155.68</t>
+          <t>28590.00</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>267.43</t>
+          <t>1672.52</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>28820255000110</t>
+          <t>12805036000121</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8767</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>17022</t>
+          <t>17003</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>8632.30</t>
+          <t>27507.17</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>189.91</t>
+          <t>1609.17</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>29308439000168</t>
+          <t>12805036000121</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2255,83 +2255,83 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17004</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1408.60</t>
+          <t>246677.04</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>82.40</t>
+          <t>14430.61</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>31170338000115</t>
+          <t>13231916000102</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>949.90</t>
+          <t>327.09</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>55.57</t>
+          <t>4.06</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>33919741000120</t>
+          <t>13653008000107</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>17023</t>
+          <t>17009</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13459.46</t>
+          <t>990.00</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>948.97</t>
+          <t>57.92</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>33919741000120</t>
+          <t>13938438000167</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6175</t>
+          <t>6147</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2341,19 +2341,19 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>992.61</t>
+          <t>20618.25</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>69.96</t>
+          <t>1206.17</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>34331544000158</t>
+          <t>14522178000107</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2368,201 +2368,1686 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>46.98</t>
+          <t>28.85</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3.31</t>
+          <t>2.03</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>42262411000103</t>
+          <t>14639720000106</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6175</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2160.08</t>
+          <t>36.27</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>126.37</t>
+          <t>2.56</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>43684445000140</t>
+          <t>15559082000186</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6175</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1205.36</t>
+          <t>177.06</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>266.59</t>
+          <t>12.48</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>54565478000198</t>
+          <t>15578569000106</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6175</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>22400.00</t>
+          <t>214.55</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1310.40</t>
+          <t>15.12</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>59717553000617</t>
+          <t>16180804000150</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>4140.00</t>
+          <t>330.04</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>242.19</t>
+          <t>4.09</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>61461034000178</t>
+          <t>16951665000110</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>6147</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17009</t>
+          <t>17099</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1500.00</t>
+          <t>460.00</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>87.75</t>
+          <t>43.47</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>64799539000135</t>
+          <t>17018886000101</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>6190</t>
+          <t>8739</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17035</t>
+          <t>17013</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>123652.48</t>
+          <t>315.10</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>11685.16</t>
+          <t>3.91</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>87883807000106</t>
+          <t>17086031000100</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>6188</t>
+          <t>6190</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>17027</t>
+          <t>17032</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>3903.20</t>
+          <t>238690.17</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>275.18</t>
+          <t>22556.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>17654293000123</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>361.40</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>4.48</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>18301321000191</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>17033</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>18035.88</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>1704.39</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>18607653000107</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>17099</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>21348.00</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>1248.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>19674909000153</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>30.40</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2.14</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>19726111000108</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>83.60</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>5.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>20982406000124</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>8469.68</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>495.48</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>20982406000124</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>93464.84</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>8832.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>20982406000124</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>17099</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>169800.00</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>16046.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>21265217000101</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>208.85</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>21306287000152</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>10800.00</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>631.80</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>22022155000161</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>17099</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>245.00</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>23.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>22524403000172</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>1256.70</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>15.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>22566069000110</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>17001</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>553.95</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>32.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>23669246000156</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>115.00</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>6.73</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>23669246000156</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>17099</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>440.00</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>41.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>24396327000192</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>17004</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>177552.48</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>10386.82</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>27059460000141</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>106.28</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>7.49</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>27059565000109</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>48.71</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>3.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>27183604000177</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2021.00</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>118.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>27729308000129</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>17001</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>8033.88</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>469.98</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>27729308000129</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2184.06</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>127.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>27729308000129</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>8767</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>17001</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>133.50</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2.94</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>27844178000175</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>48.40</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>3.41</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>27950582000123</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>126.27</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>8.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>28584157000392</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>64870.00</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>3794.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>28820255000110</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>8767</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>17008</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>836.40</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>18.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>28820255000110</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>8767</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>17022</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>190012.23</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>4180.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>30285425000155</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>139.58</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>31143966000101</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>858.12</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>10.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>31731853000127</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>7700.00</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>450.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>33013988000182</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>6256</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>200.00</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>3.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>33919741000120</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>3661.71</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>258.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>33919741000120</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>17099</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>158.22</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>34028316002157</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>17030</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>3806.42</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>176.98</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>34192524000143</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>7492.40</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>438.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>35593870000104</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>13099.98</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>162.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>35808926000192</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>405.05</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>5.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>36056645000193</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>905.38</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>11.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>36081955000168</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>840.13</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>10.42</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>40432544000147</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>17029</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>4033.95</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>381.21</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>41057571000140</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>1542.85</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>19.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>41057571000301</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>656.25</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>8.14</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>41106188000304</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>17001</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>540077.80</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>31594.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>42130537000116</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>42.76</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>42206269000179</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>6175</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>17023</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>41.53</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>42262411000103</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>3238.17</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>189.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>43684445000140</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>1845.10</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>107.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>46218314000166</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>1800.00</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>105.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>64799539000135</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>6190</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>17035</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>121400.48</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>11472.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>65149197000251</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>9140.00</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>534.69</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>70184056000129</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>8739</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>17013</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>422.44</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>5.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>74161373000180</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>17099</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>12320.00</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>720.72</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>81243735001977</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>17009</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>71140.00</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>4161.69</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>81243735001977</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>17022</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>49798.00</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>1095.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>81243735001977</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>8767</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>17022</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>3557.00</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>78.25</t>
         </is>
       </c>
     </row>

</xml_diff>